<commit_message>
adaptação do código de previsao e novos resultados
</commit_message>
<xml_diff>
--- a/CryptoRush/Codigo/Resultados testes parametros/Bitcoin - Média resultado geral.xlsx
+++ b/CryptoRush/Codigo/Resultados testes parametros/Bitcoin - Média resultado geral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yupopic\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arq. Andrea\Documents\Yuri\git\TCC-CryptoRush\CryptoRush\Codigo\Resultados testes parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982C19F2-95EC-40CA-AD1A-F9F67AFDE918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4A678B-C7E0-4E3D-823F-245C80D95CBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,20 +408,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
@@ -467,7 +467,7 @@
         <v>92.825666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>60</v>
       </c>
@@ -490,7 +490,7 @@
         <v>92.497</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>90</v>
       </c>
@@ -513,7 +513,7 @@
         <v>92.426999999999992</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80</v>
       </c>
@@ -536,7 +536,7 @@
         <v>92.37166666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>70</v>
       </c>
@@ -559,7 +559,7 @@
         <v>92.332000000000008</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>50</v>
       </c>
@@ -582,7 +582,7 @@
         <v>91.714666666666673</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>100</v>
       </c>
@@ -605,7 +605,7 @@
         <v>91.480999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>90</v>
       </c>
@@ -628,7 +628,7 @@
         <v>90.259666666666661</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>80</v>
       </c>
@@ -651,7 +651,7 @@
         <v>89.916333333333327</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100</v>
       </c>
@@ -674,7 +674,7 @@
         <v>88.76466666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>70</v>
       </c>
@@ -697,7 +697,7 @@
         <v>88.51766666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>90</v>
       </c>
@@ -720,7 +720,7 @@
         <v>88.285666666666671</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>60</v>
       </c>
@@ -743,7 +743,7 @@
         <v>86.818333333333342</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>80</v>
       </c>
@@ -766,7 +766,7 @@
         <v>86.803666666666672</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>100</v>
       </c>
@@ -789,7 +789,7 @@
         <v>85.844000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>70</v>
       </c>
@@ -812,7 +812,7 @@
         <v>85.762</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>50</v>
       </c>
@@ -835,7 +835,7 @@
         <v>85.419000000000011</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>90</v>
       </c>
@@ -858,7 +858,7 @@
         <v>85.185666666666677</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>80</v>
       </c>
@@ -881,7 +881,7 @@
         <v>84.856666666666655</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>60</v>
       </c>
@@ -904,7 +904,7 @@
         <v>84.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>50</v>
       </c>
@@ -927,7 +927,7 @@
         <v>83.304666666666662</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>70</v>
       </c>
@@ -950,7 +950,7 @@
         <v>82.716333333333324</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>60</v>
       </c>
@@ -973,7 +973,7 @@
         <v>81.522999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>90</v>
       </c>
@@ -996,7 +996,7 @@
         <v>81.371000000000009</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>100</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>81.275666666666666</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>50</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>81.083333333333329</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>100</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>80.465666666666664</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>80</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>80.342666666666673</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>90</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>80.287999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>60</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>79.917666666666676</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>50</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>79.725333333333339</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>70</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>79.670666666666662</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>100</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>79.630333333333326</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>100</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>79.587333333333333</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>60</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>79.464333333333329</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>70</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>79.438666666666663</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>90</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>79.423999999999992</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>80</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>79.355000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>80</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>79.190666666666658</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>80</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>79.135999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>70</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>79.12166666666667</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>50</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>79.026666666666671</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>90</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>79.01166666666667</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>60</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>78.957333333333324</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>90</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>78.751999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>100</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>78.737666666666669</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>50</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>78.519000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>100</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>78.503999999999991</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>70</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>78.450666666666663</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>70</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>78.368333333333339</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>80</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>78.271000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>90</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>78.243333333333339</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>80</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>77.942000000000007</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>100</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>77.928666666666672</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>50</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>77.366</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>60</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>77.338333333333338</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>100</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>77.283333333333331</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>70</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>77.25633333333333</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>60</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>77.215333333333334</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>90</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>77.214333333333329</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>76.789666666666662</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>100</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>76.680000000000007</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>50</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>76.679333333333332</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>80</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>76.487666666666669</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>90</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>76.39200000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>90</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>76.336333333333343</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>100</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>76.323333333333323</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>80</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>76.213333333333338</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>80</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>76.077666666666659</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>90</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>76.076999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>75.912000000000006</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>60</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>75.88366666666667</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>50</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>75.816333333333333</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>90</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>75.679333333333332</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>100</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>75.679333333333332</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>70</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>75.666333333333327</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>100</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>75.583000000000013</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>70</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>75.488</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>60</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>75.473333333333329</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>75.460000000000008</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>70</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>75.021000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>80</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>74.953333333333333</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>100</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>74.953000000000003</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>90</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>74.939333333333323</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>60</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>74.86999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>80</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>74.843000000000004</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>50</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>74.840999999999994</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>100</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>74.828999999999994</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>90</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>74.801666666666677</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>70</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>74.733666666666679</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>50</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>74.472333333333339</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>90</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>74.471999999999994</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>70</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>74.335666666666668</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>60</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>74.28</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>50</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>74.266333333333321</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>80</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>74.00566666666667</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>70</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>73.965666666666678</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>80</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>73.964999999999989</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>60</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>73.730666666666664</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>60</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>73.634666666666661</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>73.594000000000008</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>70</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>73.525666666666666</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>90</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>73.23833333333333</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>50</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>73.182666666666663</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>50</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>72.976333333333329</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>80</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>72.703000000000003</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>60</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>72.661000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>50</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>72.481999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>60</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>72.400333333333322</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>100</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>72.332333333333324</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>70</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>72.209666666666664</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>100</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>72.071666666666673</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>50</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>71.92</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>90</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>71.852333333333334</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>90</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>71.714333333333329</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>80</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>71.700333333333347</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>100</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>71.646666666666675</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>50</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>71.495666666666665</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>60</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>71.290333333333336</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>100</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>70.959666666666664</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>90</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>70.918666666666667</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>80</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>70.808999999999997</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>70</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>70.50633333333333</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>70</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>70.424666666666653</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>90</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>70.177666666666667</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>50</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>70.041666666666671</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>80</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>69.930666666666667</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>100</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>69.89</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>60</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>69.616</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>70</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>69.25833333333334</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>80</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>69.108333333333334</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>90</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>68.971000000000004</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>60</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>68.73833333333333</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>50</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>68.56</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>80</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>68.545666666666662</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>60</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>68.449666666666658</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>70</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>68.449666666666658</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>60</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>68.395666666666656</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>50</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>68.353999999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>50</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>68.066000000000003</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>70</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>67.847333333333324</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>60</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>67.229333333333344</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>50</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>67.024666666666661</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>50</v>
       </c>

</xml_diff>